<commit_message>
FMX-1024: Fix clash with ABP id by regeneration.
</commit_message>
<xml_diff>
--- a/apps/resources/categories_mapping.xlsx
+++ b/apps/resources/categories_mapping.xlsx
@@ -41,12 +41,15 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'categories-sous categories'!$A$1:$P$144</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">'categories-sous categories'!$A$1:$P$144</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">'categories-sous categories'!$A$1:$P$144</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'categories-sous categories'!$A$1:$P$144</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles" vbProcedure="false">'categories-sous categories'!$1:$2</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0" vbProcedure="false">'categories-sous categories'!$1:$2</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0" vbProcedure="false">'categories-sous categories'!$1:$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0" vbProcedure="false">'categories-sous categories'!$1:$2</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'categories-sous categories'!$A$2:$Q$144</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">'categories-sous categories'!$A$2:$Q$144</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'categories-sous categories'!$A$2:$Q$144</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'categories-sous categories'!$A$2:$Q$144</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -883,34 +886,34 @@
   </sheetPr>
   <dimension ref="A1:Y65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="W164" activeCellId="0" sqref="W164"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A185" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I204" activeCellId="0" sqref="I204"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="22.8178137651822"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="32.1376518218623"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="36.8502024291498"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="22.9230769230769"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="32.3481781376518"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="37.17004048583"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="10.7125506072875"/>
     <col collapsed="false" hidden="false" max="7" min="6" style="1" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="1" width="10.7125506072875"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="1" width="8.89068825910931"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="12.3198380566802"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="12.4251012145749"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="2" width="0.8582995951417"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="1" width="13.7125506072874"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="20.7813765182186"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="19.6032388663968"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="20.8866396761134"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="19.7085020242915"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="1" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="16" min="16" style="1" width="10.7125506072875"/>
     <col collapsed="false" hidden="false" max="17" min="17" style="3" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="18" min="18" style="3" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="3" width="12.8542510121458"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="3" width="12.9595141700405"/>
     <col collapsed="false" hidden="false" max="20" min="20" style="3" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="21" min="21" style="3" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="12.3198380566802"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="15.3198380566802"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="12.4251012145749"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="15.4251012145749"/>
     <col collapsed="false" hidden="false" max="24" min="24" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="25" style="0" width="8.57085020242915"/>
   </cols>
@@ -8726,7 +8729,7 @@
         <v>1</v>
       </c>
       <c r="I145" s="1" t="n">
-        <v>160</v>
+        <v>192</v>
       </c>
       <c r="J145" s="0"/>
       <c r="L145" s="1" t="s">
@@ -8775,7 +8778,7 @@
         <v>1</v>
       </c>
       <c r="I146" s="1" t="n">
-        <v>158</v>
+        <v>190</v>
       </c>
       <c r="J146" s="0"/>
       <c r="L146" s="1" t="s">
@@ -8825,7 +8828,7 @@
         <v>2</v>
       </c>
       <c r="I147" s="1" t="n">
-        <v>161</v>
+        <v>193</v>
       </c>
       <c r="J147" s="0"/>
       <c r="L147" s="1" t="s">
@@ -8876,7 +8879,7 @@
         <v>2</v>
       </c>
       <c r="I148" s="1" t="n">
-        <v>159</v>
+        <v>191</v>
       </c>
       <c r="J148" s="0"/>
       <c r="L148" s="1" t="s">
@@ -8927,7 +8930,7 @@
         <v>2</v>
       </c>
       <c r="I149" s="1" t="n">
-        <v>165</v>
+        <v>197</v>
       </c>
       <c r="J149" s="0"/>
       <c r="L149" s="1" t="s">
@@ -8976,7 +8979,7 @@
         <v>2</v>
       </c>
       <c r="I150" s="1" t="n">
-        <v>163</v>
+        <v>195</v>
       </c>
       <c r="J150" s="0"/>
       <c r="L150" s="1" t="s">
@@ -9025,7 +9028,7 @@
         <v>2</v>
       </c>
       <c r="I151" s="1" t="n">
-        <v>173</v>
+        <v>205</v>
       </c>
       <c r="J151" s="0"/>
       <c r="L151" s="1" t="s">
@@ -9075,7 +9078,7 @@
         <v>2</v>
       </c>
       <c r="I152" s="1" t="n">
-        <v>171</v>
+        <v>203</v>
       </c>
       <c r="J152" s="0"/>
       <c r="L152" s="1" t="s">
@@ -9125,7 +9128,7 @@
         <v>2</v>
       </c>
       <c r="I153" s="1" t="n">
-        <v>149</v>
+        <v>181</v>
       </c>
       <c r="J153" s="0"/>
       <c r="L153" s="1" t="s">
@@ -9168,7 +9171,7 @@
         <v>2</v>
       </c>
       <c r="I154" s="1" t="n">
-        <v>145</v>
+        <v>177</v>
       </c>
       <c r="J154" s="0"/>
       <c r="L154" s="1" t="s">
@@ -9218,7 +9221,7 @@
         <v>2</v>
       </c>
       <c r="I155" s="1" t="n">
-        <v>143</v>
+        <v>175</v>
       </c>
       <c r="J155" s="0"/>
       <c r="L155" s="1" t="s">
@@ -9269,7 +9272,7 @@
         <v>2</v>
       </c>
       <c r="I156" s="1" t="n">
-        <v>141</v>
+        <v>173</v>
       </c>
       <c r="J156" s="0"/>
       <c r="L156" s="1" t="s">
@@ -9322,7 +9325,7 @@
         <v>2</v>
       </c>
       <c r="I157" s="1" t="n">
-        <v>139</v>
+        <v>171</v>
       </c>
       <c r="J157" s="0"/>
       <c r="L157" s="1" t="s">
@@ -9378,7 +9381,7 @@
         <v>1</v>
       </c>
       <c r="I158" s="1" t="n">
-        <v>172</v>
+        <v>204</v>
       </c>
       <c r="J158" s="0"/>
       <c r="L158" s="1" t="s">
@@ -9431,7 +9434,7 @@
         <v>1</v>
       </c>
       <c r="I159" s="1" t="n">
-        <v>170</v>
+        <v>202</v>
       </c>
       <c r="J159" s="0"/>
       <c r="L159" s="1" t="s">
@@ -9482,7 +9485,7 @@
         <v>1</v>
       </c>
       <c r="I160" s="1" t="n">
-        <v>148</v>
+        <v>180</v>
       </c>
       <c r="J160" s="0"/>
       <c r="L160" s="1" t="s">
@@ -9527,7 +9530,7 @@
         <v>1</v>
       </c>
       <c r="I161" s="1" t="n">
-        <v>144</v>
+        <v>176</v>
       </c>
       <c r="J161" s="0"/>
       <c r="L161" s="1" t="s">
@@ -9578,7 +9581,7 @@
         <v>1</v>
       </c>
       <c r="I162" s="1" t="n">
-        <v>142</v>
+        <v>174</v>
       </c>
       <c r="J162" s="0"/>
       <c r="L162" s="1" t="s">
@@ -9629,7 +9632,7 @@
         <v>1</v>
       </c>
       <c r="I163" s="1" t="n">
-        <v>140</v>
+        <v>172</v>
       </c>
       <c r="J163" s="0"/>
       <c r="L163" s="1" t="s">
@@ -9685,7 +9688,7 @@
         <v>1</v>
       </c>
       <c r="I164" s="1" t="n">
-        <v>138</v>
+        <v>170</v>
       </c>
       <c r="J164" s="0"/>
       <c r="L164" s="1" t="s">
@@ -9741,7 +9744,7 @@
         <v>2</v>
       </c>
       <c r="I165" s="1" t="n">
-        <v>135</v>
+        <v>167</v>
       </c>
       <c r="J165" s="0"/>
       <c r="L165" s="1" t="s">
@@ -9790,7 +9793,7 @@
         <v>2</v>
       </c>
       <c r="I166" s="1" t="n">
-        <v>131</v>
+        <v>163</v>
       </c>
       <c r="J166" s="0"/>
       <c r="L166" s="1" t="s">
@@ -9840,7 +9843,7 @@
         <v>2</v>
       </c>
       <c r="I167" s="1" t="n">
-        <v>129</v>
+        <v>161</v>
       </c>
       <c r="J167" s="0"/>
       <c r="L167" s="1" t="s">
@@ -9890,7 +9893,7 @@
         <v>2</v>
       </c>
       <c r="I168" s="1" t="n">
-        <v>127</v>
+        <v>159</v>
       </c>
       <c r="J168" s="0"/>
       <c r="L168" s="1" t="s">
@@ -9940,7 +9943,7 @@
         <v>1</v>
       </c>
       <c r="I169" s="1" t="n">
-        <v>134</v>
+        <v>166</v>
       </c>
       <c r="J169" s="0"/>
       <c r="L169" s="1" t="s">
@@ -9991,7 +9994,7 @@
         <v>1</v>
       </c>
       <c r="I170" s="1" t="n">
-        <v>130</v>
+        <v>162</v>
       </c>
       <c r="J170" s="0"/>
       <c r="L170" s="1" t="s">
@@ -10042,7 +10045,7 @@
         <v>1</v>
       </c>
       <c r="I171" s="1" t="n">
-        <v>128</v>
+        <v>160</v>
       </c>
       <c r="J171" s="0"/>
       <c r="L171" s="1" t="s">
@@ -10093,7 +10096,7 @@
         <v>1</v>
       </c>
       <c r="I172" s="1" t="n">
-        <v>126</v>
+        <v>158</v>
       </c>
       <c r="J172" s="0"/>
       <c r="L172" s="1" t="s">
@@ -10147,7 +10150,7 @@
         <v>2</v>
       </c>
       <c r="I173" s="1" t="n">
-        <v>125</v>
+        <v>157</v>
       </c>
       <c r="J173" s="1" t="n">
         <v>1</v>
@@ -10213,7 +10216,7 @@
       </c>
       <c r="I174" s="1" t="n">
         <f aca="false">I173</f>
-        <v>125</v>
+        <v>157</v>
       </c>
       <c r="J174" s="1" t="n">
         <v>2</v>
@@ -10279,7 +10282,7 @@
       </c>
       <c r="I175" s="1" t="n">
         <f aca="false">I174</f>
-        <v>125</v>
+        <v>157</v>
       </c>
       <c r="J175" s="1" t="n">
         <v>3</v>
@@ -10345,7 +10348,7 @@
       </c>
       <c r="I176" s="1" t="n">
         <f aca="false">I175</f>
-        <v>125</v>
+        <v>157</v>
       </c>
       <c r="J176" s="1" t="n">
         <v>4</v>
@@ -10411,7 +10414,7 @@
       </c>
       <c r="I177" s="1" t="n">
         <f aca="false">I176</f>
-        <v>125</v>
+        <v>157</v>
       </c>
       <c r="J177" s="1" t="n">
         <v>5</v>
@@ -10477,7 +10480,7 @@
       </c>
       <c r="I178" s="1" t="n">
         <f aca="false">I177</f>
-        <v>125</v>
+        <v>157</v>
       </c>
       <c r="J178" s="1" t="n">
         <v>6</v>
@@ -10541,7 +10544,7 @@
         <v>1</v>
       </c>
       <c r="I179" s="1" t="n">
-        <v>124</v>
+        <v>156</v>
       </c>
       <c r="J179" s="1" t="n">
         <v>1</v>
@@ -10607,7 +10610,7 @@
       </c>
       <c r="I180" s="1" t="n">
         <f aca="false">I179</f>
-        <v>124</v>
+        <v>156</v>
       </c>
       <c r="J180" s="1" t="n">
         <v>2</v>
@@ -10673,7 +10676,7 @@
       </c>
       <c r="I181" s="1" t="n">
         <f aca="false">I180</f>
-        <v>124</v>
+        <v>156</v>
       </c>
       <c r="J181" s="1" t="n">
         <v>3</v>
@@ -10739,7 +10742,7 @@
       </c>
       <c r="I182" s="1" t="n">
         <f aca="false">I181</f>
-        <v>124</v>
+        <v>156</v>
       </c>
       <c r="J182" s="1" t="n">
         <v>4</v>
@@ -10805,7 +10808,7 @@
       </c>
       <c r="I183" s="1" t="n">
         <f aca="false">I182</f>
-        <v>124</v>
+        <v>156</v>
       </c>
       <c r="J183" s="1" t="n">
         <v>5</v>
@@ -10871,7 +10874,7 @@
       </c>
       <c r="I184" s="1" t="n">
         <f aca="false">I183</f>
-        <v>124</v>
+        <v>156</v>
       </c>
       <c r="J184" s="1" t="n">
         <v>6</v>
@@ -10935,7 +10938,7 @@
         <v>2</v>
       </c>
       <c r="I185" s="1" t="n">
-        <v>123</v>
+        <v>155</v>
       </c>
       <c r="J185" s="1" t="n">
         <v>1</v>
@@ -11000,7 +11003,7 @@
       </c>
       <c r="I186" s="1" t="n">
         <f aca="false">I185</f>
-        <v>123</v>
+        <v>155</v>
       </c>
       <c r="J186" s="1" t="n">
         <v>2</v>
@@ -11066,7 +11069,7 @@
       </c>
       <c r="I187" s="1" t="n">
         <f aca="false">I186</f>
-        <v>123</v>
+        <v>155</v>
       </c>
       <c r="J187" s="1" t="n">
         <v>3</v>
@@ -11132,7 +11135,7 @@
       </c>
       <c r="I188" s="1" t="n">
         <f aca="false">I187</f>
-        <v>123</v>
+        <v>155</v>
       </c>
       <c r="J188" s="1" t="n">
         <v>4</v>
@@ -11198,7 +11201,7 @@
       </c>
       <c r="I189" s="1" t="n">
         <f aca="false">I188</f>
-        <v>123</v>
+        <v>155</v>
       </c>
       <c r="J189" s="1" t="n">
         <v>5</v>
@@ -11264,7 +11267,7 @@
       </c>
       <c r="I190" s="1" t="n">
         <f aca="false">I189</f>
-        <v>123</v>
+        <v>155</v>
       </c>
       <c r="J190" s="1" t="n">
         <v>6</v>
@@ -11328,7 +11331,7 @@
         <v>1</v>
       </c>
       <c r="I191" s="1" t="n">
-        <v>122</v>
+        <v>154</v>
       </c>
       <c r="J191" s="1" t="n">
         <v>1</v>
@@ -11394,7 +11397,7 @@
       </c>
       <c r="I192" s="1" t="n">
         <f aca="false">I191</f>
-        <v>122</v>
+        <v>154</v>
       </c>
       <c r="J192" s="1" t="n">
         <v>2</v>
@@ -11460,7 +11463,7 @@
       </c>
       <c r="I193" s="1" t="n">
         <f aca="false">I192</f>
-        <v>122</v>
+        <v>154</v>
       </c>
       <c r="J193" s="1" t="n">
         <v>3</v>
@@ -11526,7 +11529,7 @@
       </c>
       <c r="I194" s="1" t="n">
         <f aca="false">I193</f>
-        <v>122</v>
+        <v>154</v>
       </c>
       <c r="J194" s="1" t="n">
         <v>4</v>
@@ -11592,7 +11595,7 @@
       </c>
       <c r="I195" s="1" t="n">
         <f aca="false">I194</f>
-        <v>122</v>
+        <v>154</v>
       </c>
       <c r="J195" s="1" t="n">
         <v>5</v>
@@ -11658,7 +11661,7 @@
       </c>
       <c r="I196" s="1" t="n">
         <f aca="false">I195</f>
-        <v>122</v>
+        <v>154</v>
       </c>
       <c r="J196" s="1" t="n">
         <v>6</v>
@@ -11722,7 +11725,7 @@
         <v>2</v>
       </c>
       <c r="I197" s="1" t="n">
-        <v>121</v>
+        <v>153</v>
       </c>
       <c r="J197" s="1" t="n">
         <v>1</v>
@@ -11788,7 +11791,7 @@
       </c>
       <c r="I198" s="1" t="n">
         <f aca="false">I197</f>
-        <v>121</v>
+        <v>153</v>
       </c>
       <c r="J198" s="1" t="n">
         <v>2</v>
@@ -11854,7 +11857,7 @@
       </c>
       <c r="I199" s="1" t="n">
         <f aca="false">I198</f>
-        <v>121</v>
+        <v>153</v>
       </c>
       <c r="J199" s="1" t="n">
         <v>3</v>
@@ -11920,7 +11923,7 @@
       </c>
       <c r="I200" s="1" t="n">
         <f aca="false">I199</f>
-        <v>121</v>
+        <v>153</v>
       </c>
       <c r="J200" s="1" t="n">
         <v>4</v>
@@ -11986,7 +11989,7 @@
       </c>
       <c r="I201" s="1" t="n">
         <f aca="false">I200</f>
-        <v>121</v>
+        <v>153</v>
       </c>
       <c r="J201" s="1" t="n">
         <v>5</v>
@@ -12052,7 +12055,7 @@
       </c>
       <c r="I202" s="1" t="n">
         <f aca="false">I201</f>
-        <v>121</v>
+        <v>153</v>
       </c>
       <c r="J202" s="1" t="n">
         <v>6</v>
@@ -12116,7 +12119,7 @@
         <v>1</v>
       </c>
       <c r="I203" s="1" t="n">
-        <v>120</v>
+        <v>152</v>
       </c>
       <c r="J203" s="1" t="n">
         <v>1</v>
@@ -12182,7 +12185,7 @@
       </c>
       <c r="I204" s="1" t="n">
         <f aca="false">I203</f>
-        <v>120</v>
+        <v>152</v>
       </c>
       <c r="J204" s="1" t="n">
         <v>2</v>
@@ -12248,7 +12251,7 @@
       </c>
       <c r="I205" s="1" t="n">
         <f aca="false">I204</f>
-        <v>120</v>
+        <v>152</v>
       </c>
       <c r="J205" s="1" t="n">
         <v>3</v>
@@ -12314,7 +12317,7 @@
       </c>
       <c r="I206" s="1" t="n">
         <f aca="false">I205</f>
-        <v>120</v>
+        <v>152</v>
       </c>
       <c r="J206" s="1" t="n">
         <v>4</v>
@@ -12380,7 +12383,7 @@
       </c>
       <c r="I207" s="1" t="n">
         <f aca="false">I206</f>
-        <v>120</v>
+        <v>152</v>
       </c>
       <c r="J207" s="1" t="n">
         <v>5</v>
@@ -12446,7 +12449,7 @@
       </c>
       <c r="I208" s="1" t="n">
         <f aca="false">I207</f>
-        <v>120</v>
+        <v>152</v>
       </c>
       <c r="J208" s="1" t="n">
         <v>6</v>

</xml_diff>

<commit_message>
FMX-1030: Fix categories mapping
</commit_message>
<xml_diff>
--- a/apps/resources/categories_mapping.xlsx
+++ b/apps/resources/categories_mapping.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="categories-sous categories" sheetId="1" state="visible" r:id="rId2"/>
@@ -42,14 +42,17 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">'categories-sous categories'!$A$1:$P$144</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">'categories-sous categories'!$A$1:$P$144</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'categories-sous categories'!$A$1:$P$144</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'categories-sous categories'!$A$1:$P$144</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles" vbProcedure="false">'categories-sous categories'!$1:$2</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0" vbProcedure="false">'categories-sous categories'!$1:$2</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0" vbProcedure="false">'categories-sous categories'!$1:$2</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0" vbProcedure="false">'categories-sous categories'!$1:$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0" vbProcedure="false">'categories-sous categories'!$1:$2</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'categories-sous categories'!$A$2:$Q$144</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">'categories-sous categories'!$A$2:$Q$144</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'categories-sous categories'!$A$2:$Q$144</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'categories-sous categories'!$A$2:$Q$144</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">'categories-sous categories'!$A$2:$Q$144</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -61,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1495" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1495" uniqueCount="167">
   <si>
     <t xml:space="preserve">Anicennes catégories</t>
   </si>
@@ -351,7 +354,7 @@
     <t xml:space="preserve">Avaloir </t>
   </si>
   <si>
-    <t xml:space="preserve">bouché</t>
+    <t xml:space="preserve">Avaloir bouché</t>
   </si>
   <si>
     <t xml:space="preserve">Grille manquante</t>
@@ -439,9 +442,6 @@
   </si>
   <si>
     <t xml:space="preserve">bouchage ordinaire</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Avaloir bouché</t>
   </si>
   <si>
     <t xml:space="preserve">Dépôts clandestins</t>
@@ -574,7 +574,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -619,6 +619,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="9">
@@ -737,7 +743,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -798,7 +804,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -886,34 +904,34 @@
   </sheetPr>
   <dimension ref="A1:Y65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A185" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I204" activeCellId="0" sqref="I204"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J128" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="U150" activeCellId="0" sqref="U150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="22.9230769230769"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="32.3481781376518"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="37.17004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="32.5627530364372"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="37.4898785425101"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="10.7125506072875"/>
     <col collapsed="false" hidden="false" max="7" min="6" style="1" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="1" width="10.7125506072875"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="1" width="8.89068825910931"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="12.4251012145749"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="12.5344129554656"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="2" width="0.8582995951417"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="1" width="13.7125506072874"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="20.8866396761134"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="20.995951417004"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="19.8178137651822"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="1" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="16" min="16" style="1" width="10.7125506072875"/>
     <col collapsed="false" hidden="false" max="17" min="17" style="3" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="18" min="18" style="3" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="3" width="12.9595141700405"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="3" width="13.0688259109312"/>
     <col collapsed="false" hidden="false" max="20" min="20" style="3" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="21" min="21" style="3" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="12.4251012145749"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="12.5344129554656"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="15.5303643724696"/>
     <col collapsed="false" hidden="false" max="24" min="24" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="25" style="0" width="8.57085020242915"/>
   </cols>
@@ -4648,9 +4666,9 @@
         <f aca="false">S63</f>
         <v>2020</v>
       </c>
-      <c r="T67" s="12" t="n">
-        <f aca="false">I67+3000</f>
-        <v>3096</v>
+      <c r="T67" s="15" t="n">
+        <f aca="false">T63</f>
+        <v>3049</v>
       </c>
       <c r="U67" s="0"/>
     </row>
@@ -4703,7 +4721,7 @@
       </c>
       <c r="T68" s="3" t="n">
         <f aca="false">T67</f>
-        <v>3096</v>
+        <v>3049</v>
       </c>
       <c r="U68" s="0"/>
     </row>
@@ -4756,7 +4774,7 @@
       </c>
       <c r="T69" s="3" t="n">
         <f aca="false">T67</f>
-        <v>3096</v>
+        <v>3049</v>
       </c>
       <c r="U69" s="0"/>
     </row>
@@ -5689,7 +5707,7 @@
       <c r="M87" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="N87" s="15" t="s">
+      <c r="N87" s="16" t="s">
         <v>87</v>
       </c>
       <c r="O87" s="0"/>
@@ -5741,7 +5759,7 @@
       <c r="M88" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="N88" s="15" t="s">
+      <c r="N88" s="16" t="s">
         <v>89</v>
       </c>
       <c r="O88" s="0"/>
@@ -5793,7 +5811,7 @@
       <c r="M89" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="N89" s="15" t="s">
+      <c r="N89" s="16" t="s">
         <v>91</v>
       </c>
       <c r="O89" s="0"/>
@@ -5845,7 +5863,7 @@
       <c r="M90" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="N90" s="15" t="s">
+      <c r="N90" s="16" t="s">
         <v>92</v>
       </c>
       <c r="O90" s="0"/>
@@ -5898,7 +5916,7 @@
       <c r="M91" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="N91" s="15" t="s">
+      <c r="N91" s="16" t="s">
         <v>89</v>
       </c>
       <c r="O91" s="0"/>
@@ -5951,7 +5969,7 @@
       <c r="M92" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="N92" s="15" t="s">
+      <c r="N92" s="16" t="s">
         <v>91</v>
       </c>
       <c r="O92" s="0"/>
@@ -6004,7 +6022,7 @@
       <c r="M93" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="N93" s="15" t="s">
+      <c r="N93" s="16" t="s">
         <v>89</v>
       </c>
       <c r="O93" s="0"/>
@@ -6057,7 +6075,7 @@
       <c r="M94" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="N94" s="15" t="s">
+      <c r="N94" s="16" t="s">
         <v>91</v>
       </c>
       <c r="O94" s="0"/>
@@ -6110,7 +6128,7 @@
       <c r="M95" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="N95" s="15" t="s">
+      <c r="N95" s="16" t="s">
         <v>92</v>
       </c>
       <c r="O95" s="0"/>
@@ -6163,7 +6181,7 @@
       <c r="M96" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="N96" s="15" t="s">
+      <c r="N96" s="16" t="s">
         <v>91</v>
       </c>
       <c r="O96" s="0"/>
@@ -6216,7 +6234,7 @@
       <c r="M97" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="N97" s="15" t="s">
+      <c r="N97" s="16" t="s">
         <v>92</v>
       </c>
       <c r="O97" s="0"/>
@@ -6269,7 +6287,7 @@
       <c r="M98" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="N98" s="15" t="s">
+      <c r="N98" s="16" t="s">
         <v>89</v>
       </c>
       <c r="O98" s="0"/>
@@ -6319,10 +6337,10 @@
       <c r="L99" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="M99" s="1" t="s">
+      <c r="M99" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="N99" s="15" t="s">
+      <c r="N99" s="18" t="s">
         <v>96</v>
       </c>
       <c r="O99" s="0"/>
@@ -6374,7 +6392,7 @@
       <c r="M100" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="N100" s="15" t="s">
+      <c r="N100" s="16" t="s">
         <v>97</v>
       </c>
       <c r="O100" s="0"/>
@@ -6426,7 +6444,7 @@
       <c r="M101" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="N101" s="15" t="s">
+      <c r="N101" s="16" t="s">
         <v>100</v>
       </c>
       <c r="O101" s="0"/>
@@ -6474,11 +6492,11 @@
       <c r="L102" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="M102" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="N102" s="15" t="s">
-        <v>94</v>
+      <c r="M102" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="N102" s="18" t="s">
+        <v>96</v>
       </c>
       <c r="O102" s="0"/>
       <c r="P102" s="0"/>
@@ -6530,7 +6548,7 @@
       <c r="M103" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="N103" s="15" t="s">
+      <c r="N103" s="16" t="s">
         <v>97</v>
       </c>
       <c r="O103" s="0"/>
@@ -6580,11 +6598,11 @@
       <c r="L104" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="M104" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="N104" s="15" t="s">
-        <v>94</v>
+      <c r="M104" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="N104" s="18" t="s">
+        <v>96</v>
       </c>
       <c r="O104" s="0"/>
       <c r="P104" s="0"/>
@@ -6636,7 +6654,7 @@
       <c r="M105" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="N105" s="15" t="s">
+      <c r="N105" s="16" t="s">
         <v>97</v>
       </c>
       <c r="O105" s="0"/>
@@ -6686,11 +6704,11 @@
       <c r="L106" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="M106" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="N106" s="15" t="s">
-        <v>94</v>
+      <c r="M106" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="N106" s="18" t="s">
+        <v>96</v>
       </c>
       <c r="O106" s="0"/>
       <c r="P106" s="0"/>
@@ -6742,7 +6760,7 @@
       <c r="M107" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="N107" s="15" t="s">
+      <c r="N107" s="16" t="s">
         <v>97</v>
       </c>
       <c r="O107" s="0"/>
@@ -6792,11 +6810,11 @@
       <c r="L108" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="M108" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="N108" s="15" t="s">
-        <v>94</v>
+      <c r="M108" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="N108" s="18" t="s">
+        <v>96</v>
       </c>
       <c r="O108" s="0"/>
       <c r="P108" s="0"/>
@@ -6848,7 +6866,7 @@
       <c r="M109" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="N109" s="15" t="s">
+      <c r="N109" s="16" t="s">
         <v>97</v>
       </c>
       <c r="O109" s="0"/>
@@ -6901,7 +6919,7 @@
       <c r="M110" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="N110" s="15" t="s">
+      <c r="N110" s="16" t="s">
         <v>104</v>
       </c>
       <c r="O110" s="0"/>
@@ -6953,7 +6971,7 @@
       <c r="M111" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="N111" s="15" t="s">
+      <c r="N111" s="16" t="s">
         <v>106</v>
       </c>
       <c r="O111" s="0"/>
@@ -7005,7 +7023,7 @@
       <c r="M112" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="N112" s="15" t="s">
+      <c r="N112" s="16" t="s">
         <v>106</v>
       </c>
       <c r="O112" s="0"/>
@@ -7060,7 +7078,7 @@
       <c r="M113" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="N113" s="15" t="s">
+      <c r="N113" s="16" t="s">
         <v>104</v>
       </c>
       <c r="O113" s="0"/>
@@ -7113,7 +7131,7 @@
       <c r="M114" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="N114" s="15" t="s">
+      <c r="N114" s="16" t="s">
         <v>106</v>
       </c>
       <c r="O114" s="0"/>
@@ -7166,7 +7184,7 @@
       <c r="M115" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="N115" s="15" t="s">
+      <c r="N115" s="16" t="s">
         <v>106</v>
       </c>
       <c r="O115" s="0"/>
@@ -7221,7 +7239,7 @@
       <c r="M116" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="N116" s="15" t="s">
+      <c r="N116" s="16" t="s">
         <v>104</v>
       </c>
       <c r="O116" s="0"/>
@@ -7274,7 +7292,7 @@
       <c r="M117" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="N117" s="15" t="s">
+      <c r="N117" s="16" t="s">
         <v>106</v>
       </c>
       <c r="O117" s="0"/>
@@ -7329,7 +7347,7 @@
       <c r="M118" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="N118" s="15" t="s">
+      <c r="N118" s="16" t="s">
         <v>106</v>
       </c>
       <c r="O118" s="0"/>
@@ -7382,7 +7400,7 @@
       <c r="M119" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="N119" s="15" t="s">
+      <c r="N119" s="16" t="s">
         <v>104</v>
       </c>
       <c r="O119" s="0"/>
@@ -7435,7 +7453,7 @@
       <c r="M120" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="N120" s="15" t="s">
+      <c r="N120" s="16" t="s">
         <v>106</v>
       </c>
       <c r="O120" s="0"/>
@@ -7488,7 +7506,7 @@
       <c r="M121" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="N121" s="15" t="s">
+      <c r="N121" s="16" t="s">
         <v>106</v>
       </c>
       <c r="O121" s="0"/>
@@ -7543,7 +7561,7 @@
       <c r="M122" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="N122" s="15" t="s">
+      <c r="N122" s="16" t="s">
         <v>104</v>
       </c>
       <c r="O122" s="0"/>
@@ -7596,7 +7614,7 @@
       <c r="M123" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="N123" s="15" t="s">
+      <c r="N123" s="16" t="s">
         <v>106</v>
       </c>
       <c r="O123" s="0"/>
@@ -7649,7 +7667,7 @@
       <c r="M124" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="N124" s="15" t="s">
+      <c r="N124" s="16" t="s">
         <v>106</v>
       </c>
       <c r="O124" s="0"/>
@@ -7704,7 +7722,7 @@
       <c r="M125" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="N125" s="15" t="s">
+      <c r="N125" s="16" t="s">
         <v>110</v>
       </c>
       <c r="O125" s="0"/>
@@ -7755,7 +7773,7 @@
       <c r="M126" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="N126" s="15" t="s">
+      <c r="N126" s="16" t="s">
         <v>110</v>
       </c>
       <c r="O126" s="0"/>
@@ -7807,7 +7825,7 @@
       <c r="M127" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="N127" s="15" t="s">
+      <c r="N127" s="16" t="s">
         <v>113</v>
       </c>
       <c r="O127" s="0"/>
@@ -7858,7 +7876,7 @@
       <c r="M128" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="N128" s="15" t="s">
+      <c r="N128" s="16" t="s">
         <v>115</v>
       </c>
       <c r="O128" s="0"/>
@@ -7909,7 +7927,7 @@
       <c r="M129" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="N129" s="15" t="s">
+      <c r="N129" s="16" t="s">
         <v>110</v>
       </c>
       <c r="O129" s="0"/>
@@ -7961,7 +7979,7 @@
       <c r="M130" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="N130" s="15" t="s">
+      <c r="N130" s="16" t="s">
         <v>115</v>
       </c>
       <c r="O130" s="0"/>
@@ -8013,7 +8031,7 @@
       <c r="M131" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="N131" s="15" t="s">
+      <c r="N131" s="16" t="s">
         <v>113</v>
       </c>
       <c r="O131" s="0"/>
@@ -8065,7 +8083,7 @@
       <c r="M132" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="N132" s="15" t="s">
+      <c r="N132" s="16" t="s">
         <v>110</v>
       </c>
       <c r="O132" s="0"/>
@@ -8117,7 +8135,7 @@
       <c r="M133" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="N133" s="15" t="s">
+      <c r="N133" s="16" t="s">
         <v>110</v>
       </c>
       <c r="O133" s="0"/>
@@ -8169,7 +8187,7 @@
       <c r="M134" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="N134" s="15" t="s">
+      <c r="N134" s="16" t="s">
         <v>110</v>
       </c>
       <c r="O134" s="0"/>
@@ -8221,7 +8239,7 @@
       <c r="M135" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="N135" s="15" t="s">
+      <c r="N135" s="16" t="s">
         <v>113</v>
       </c>
       <c r="O135" s="0"/>
@@ -8273,7 +8291,7 @@
       <c r="M136" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="N136" s="15" t="s">
+      <c r="N136" s="16" t="s">
         <v>115</v>
       </c>
       <c r="O136" s="0"/>
@@ -8325,7 +8343,7 @@
       <c r="M137" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="N137" s="15" t="s">
+      <c r="N137" s="16" t="s">
         <v>113</v>
       </c>
       <c r="O137" s="0"/>
@@ -8377,7 +8395,7 @@
       <c r="M138" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="N138" s="15" t="s">
+      <c r="N138" s="16" t="s">
         <v>110</v>
       </c>
       <c r="O138" s="0"/>
@@ -8429,7 +8447,7 @@
       <c r="M139" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="N139" s="15" t="s">
+      <c r="N139" s="16" t="s">
         <v>110</v>
       </c>
       <c r="O139" s="0"/>
@@ -8481,7 +8499,7 @@
       <c r="M140" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="N140" s="15" t="s">
+      <c r="N140" s="16" t="s">
         <v>115</v>
       </c>
       <c r="O140" s="0"/>
@@ -8533,7 +8551,7 @@
       <c r="M141" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="N141" s="15" t="s">
+      <c r="N141" s="16" t="s">
         <v>110</v>
       </c>
       <c r="O141" s="0"/>
@@ -8585,7 +8603,7 @@
       <c r="M142" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="N142" s="15" t="s">
+      <c r="N142" s="16" t="s">
         <v>110</v>
       </c>
       <c r="O142" s="0"/>
@@ -8637,7 +8655,7 @@
       <c r="M143" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="N143" s="15" t="s">
+      <c r="N143" s="16" t="s">
         <v>113</v>
       </c>
       <c r="O143" s="0"/>
@@ -8689,7 +8707,7 @@
       <c r="M144" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="N144" s="15" t="s">
+      <c r="N144" s="16" t="s">
         <v>115</v>
       </c>
       <c r="O144" s="0"/>
@@ -8986,21 +9004,23 @@
         <v>95</v>
       </c>
       <c r="M150" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="N150" s="1" t="s">
-        <v>124</v>
+        <v>96</v>
+      </c>
+      <c r="N150" s="17" t="s">
+        <v>96</v>
       </c>
       <c r="O150" s="0"/>
       <c r="R150" s="3" t="n">
         <f aca="false">R149</f>
         <v>1003</v>
       </c>
-      <c r="S150" s="12" t="n">
-        <v>2202</v>
-      </c>
-      <c r="T150" s="12" t="n">
-        <v>3303</v>
+      <c r="S150" s="15" t="n">
+        <f aca="false">S99</f>
+        <v>2050</v>
+      </c>
+      <c r="T150" s="15" t="n">
+        <f aca="false">T99</f>
+        <v>3033</v>
       </c>
       <c r="U150" s="0"/>
       <c r="V150" s="0" t="n">
@@ -9012,13 +9032,13 @@
     </row>
     <row r="151" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B151" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D151" s="0"/>
       <c r="G151" s="1" t="n">
@@ -9038,7 +9058,7 @@
         <v>37</v>
       </c>
       <c r="N151" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="O151" s="0"/>
       <c r="R151" s="3" t="n">
@@ -9062,13 +9082,13 @@
     </row>
     <row r="152" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B152" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D152" s="0"/>
       <c r="G152" s="1" t="n">
@@ -9088,7 +9108,7 @@
         <v>37</v>
       </c>
       <c r="N152" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="O152" s="0"/>
       <c r="R152" s="3" t="n">
@@ -9112,13 +9132,13 @@
     </row>
     <row r="153" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B153" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D153" s="0"/>
       <c r="G153" s="1" t="n">
@@ -9135,10 +9155,10 @@
         <v>101</v>
       </c>
       <c r="M153" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="N153" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="O153" s="0"/>
       <c r="R153" s="3" t="n">
@@ -9155,13 +9175,13 @@
     </row>
     <row r="154" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B154" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D154" s="0"/>
       <c r="G154" s="1" t="n">
@@ -9181,7 +9201,7 @@
         <v>37</v>
       </c>
       <c r="N154" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="O154" s="0"/>
       <c r="R154" s="3" t="n">
@@ -9205,13 +9225,13 @@
     </row>
     <row r="155" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B155" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D155" s="0"/>
       <c r="G155" s="1" t="n">
@@ -9231,7 +9251,7 @@
         <v>27</v>
       </c>
       <c r="N155" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="O155" s="0"/>
       <c r="R155" s="3" t="n">
@@ -9256,13 +9276,13 @@
     </row>
     <row r="156" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B156" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D156" s="0"/>
       <c r="G156" s="1" t="n">
@@ -9285,7 +9305,7 @@
         <v>41</v>
       </c>
       <c r="O156" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="R156" s="3" t="n">
         <f aca="false">R3</f>
@@ -9309,13 +9329,13 @@
     </row>
     <row r="157" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B157" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D157" s="0"/>
       <c r="G157" s="1" t="n">
@@ -9338,7 +9358,7 @@
         <v>41</v>
       </c>
       <c r="O157" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="R157" s="3" t="n">
         <f aca="false">R3</f>
@@ -9365,13 +9385,13 @@
     </row>
     <row r="158" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B158" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D158" s="0"/>
       <c r="G158" s="1" t="n">
@@ -9391,7 +9411,7 @@
         <v>37</v>
       </c>
       <c r="N158" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="O158" s="0"/>
       <c r="R158" s="3" t="n">
@@ -9418,13 +9438,13 @@
     </row>
     <row r="159" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B159" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D159" s="0"/>
       <c r="G159" s="1" t="n">
@@ -9444,7 +9464,7 @@
         <v>37</v>
       </c>
       <c r="N159" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="O159" s="0"/>
       <c r="R159" s="3" t="n">
@@ -9469,13 +9489,13 @@
     </row>
     <row r="160" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B160" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D160" s="0"/>
       <c r="G160" s="1" t="n">
@@ -9492,10 +9512,10 @@
         <v>101</v>
       </c>
       <c r="M160" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="N160" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="O160" s="0"/>
       <c r="R160" s="3" t="n">
@@ -9514,13 +9534,13 @@
     </row>
     <row r="161" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B161" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D161" s="0"/>
       <c r="G161" s="1" t="n">
@@ -9540,7 +9560,7 @@
         <v>37</v>
       </c>
       <c r="N161" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="O161" s="0"/>
       <c r="R161" s="3" t="n">
@@ -9565,13 +9585,13 @@
     </row>
     <row r="162" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B162" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D162" s="0"/>
       <c r="G162" s="1" t="n">
@@ -9616,13 +9636,13 @@
     </row>
     <row r="163" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B163" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D163" s="0"/>
       <c r="G163" s="1" t="n">
@@ -9645,7 +9665,7 @@
         <v>41</v>
       </c>
       <c r="O163" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="R163" s="3" t="n">
         <f aca="false">R3</f>
@@ -9672,13 +9692,13 @@
     </row>
     <row r="164" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B164" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D164" s="0"/>
       <c r="G164" s="1" t="n">
@@ -9701,7 +9721,7 @@
         <v>41</v>
       </c>
       <c r="O164" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="R164" s="3" t="n">
         <f aca="false">R3</f>
@@ -9728,13 +9748,13 @@
     </row>
     <row r="165" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B165" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D165" s="0"/>
       <c r="G165" s="1" t="n">
@@ -9751,10 +9771,10 @@
         <v>78</v>
       </c>
       <c r="M165" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="N165" s="1" t="s">
         <v>144</v>
-      </c>
-      <c r="N165" s="1" t="s">
-        <v>145</v>
       </c>
       <c r="O165" s="0"/>
       <c r="R165" s="3" t="n">
@@ -9777,13 +9797,13 @@
     </row>
     <row r="166" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B166" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D166" s="0"/>
       <c r="G166" s="1" t="n">
@@ -9800,10 +9820,10 @@
         <v>78</v>
       </c>
       <c r="M166" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="N166" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="O166" s="0"/>
       <c r="R166" s="3" t="n">
@@ -9827,13 +9847,13 @@
     </row>
     <row r="167" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B167" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D167" s="0"/>
       <c r="G167" s="1" t="n">
@@ -9850,7 +9870,7 @@
         <v>78</v>
       </c>
       <c r="M167" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="N167" s="1" t="s">
         <v>121</v>
@@ -9877,13 +9897,13 @@
     </row>
     <row r="168" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B168" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D168" s="0"/>
       <c r="G168" s="1" t="n">
@@ -9900,10 +9920,10 @@
         <v>78</v>
       </c>
       <c r="M168" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="N168" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="O168" s="0"/>
       <c r="R168" s="3" t="n">
@@ -9927,13 +9947,13 @@
     </row>
     <row r="169" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B169" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D169" s="0"/>
       <c r="G169" s="1" t="n">
@@ -9950,10 +9970,10 @@
         <v>78</v>
       </c>
       <c r="M169" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="N169" s="1" t="s">
         <v>144</v>
-      </c>
-      <c r="N169" s="1" t="s">
-        <v>145</v>
       </c>
       <c r="O169" s="0"/>
       <c r="R169" s="3" t="n">
@@ -9978,13 +9998,13 @@
     </row>
     <row r="170" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B170" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D170" s="0"/>
       <c r="G170" s="1" t="n">
@@ -10001,10 +10021,10 @@
         <v>78</v>
       </c>
       <c r="M170" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="N170" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="O170" s="0"/>
       <c r="R170" s="3" t="n">
@@ -10029,13 +10049,13 @@
     </row>
     <row r="171" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B171" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D171" s="0"/>
       <c r="G171" s="1" t="n">
@@ -10052,7 +10072,7 @@
         <v>78</v>
       </c>
       <c r="M171" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="N171" s="1" t="s">
         <v>121</v>
@@ -10080,13 +10100,13 @@
     </row>
     <row r="172" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B172" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C172" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D172" s="0"/>
       <c r="G172" s="1" t="n">
@@ -10103,10 +10123,10 @@
         <v>78</v>
       </c>
       <c r="M172" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="N172" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="O172" s="0"/>
       <c r="R172" s="3" t="n">
@@ -10131,16 +10151,16 @@
     </row>
     <row r="173" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B173" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C173" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D173" s="1" t="s">
         <v>152</v>
-      </c>
-      <c r="D173" s="1" t="s">
-        <v>153</v>
       </c>
       <c r="G173" s="1" t="n">
         <f aca="false">$G$172</f>
@@ -10159,13 +10179,13 @@
         <v>20</v>
       </c>
       <c r="M173" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="N173" s="1" t="s">
         <v>43</v>
       </c>
       <c r="O173" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="R173" s="3" t="n">
         <f aca="false">R3</f>
@@ -10195,16 +10215,16 @@
     </row>
     <row r="174" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B174" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D174" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G174" s="1" t="n">
         <f aca="false">$G$172</f>
@@ -10225,13 +10245,13 @@
         <v>20</v>
       </c>
       <c r="M174" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="N174" s="1" t="s">
         <v>43</v>
       </c>
       <c r="O174" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="R174" s="3" t="n">
         <f aca="false">R3</f>
@@ -10261,16 +10281,16 @@
     </row>
     <row r="175" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B175" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C175" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D175" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G175" s="1" t="n">
         <f aca="false">$G$172</f>
@@ -10291,13 +10311,13 @@
         <v>20</v>
       </c>
       <c r="M175" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="N175" s="1" t="s">
         <v>43</v>
       </c>
       <c r="O175" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="R175" s="3" t="n">
         <f aca="false">R3</f>
@@ -10327,16 +10347,16 @@
     </row>
     <row r="176" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B176" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C176" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D176" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G176" s="1" t="n">
         <f aca="false">$G$172</f>
@@ -10357,13 +10377,13 @@
         <v>20</v>
       </c>
       <c r="M176" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="N176" s="1" t="s">
         <v>43</v>
       </c>
       <c r="O176" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="R176" s="3" t="n">
         <f aca="false">R3</f>
@@ -10393,16 +10413,16 @@
     </row>
     <row r="177" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B177" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C177" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D177" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G177" s="1" t="n">
         <f aca="false">$G$172</f>
@@ -10423,13 +10443,13 @@
         <v>20</v>
       </c>
       <c r="M177" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="N177" s="1" t="s">
         <v>43</v>
       </c>
       <c r="O177" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="R177" s="3" t="n">
         <f aca="false">R3</f>
@@ -10459,16 +10479,16 @@
     </row>
     <row r="178" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B178" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C178" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D178" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G178" s="1" t="n">
         <f aca="false">$G$172</f>
@@ -10489,13 +10509,13 @@
         <v>20</v>
       </c>
       <c r="M178" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="N178" s="1" t="s">
         <v>43</v>
       </c>
       <c r="O178" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="R178" s="3" t="n">
         <f aca="false">R3</f>
@@ -10525,16 +10545,16 @@
     </row>
     <row r="179" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B179" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C179" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D179" s="1" t="s">
         <v>152</v>
-      </c>
-      <c r="D179" s="1" t="s">
-        <v>153</v>
       </c>
       <c r="G179" s="1" t="n">
         <f aca="false">$G$172</f>
@@ -10553,13 +10573,13 @@
         <v>20</v>
       </c>
       <c r="M179" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="N179" s="1" t="s">
         <v>43</v>
       </c>
       <c r="O179" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="R179" s="3" t="n">
         <f aca="false">R3</f>
@@ -10589,16 +10609,16 @@
     </row>
     <row r="180" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B180" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C180" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D180" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G180" s="1" t="n">
         <f aca="false">$G$172</f>
@@ -10619,13 +10639,13 @@
         <v>20</v>
       </c>
       <c r="M180" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="N180" s="1" t="s">
         <v>43</v>
       </c>
       <c r="O180" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="R180" s="3" t="n">
         <f aca="false">R3</f>
@@ -10655,16 +10675,16 @@
     </row>
     <row r="181" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B181" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C181" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D181" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G181" s="1" t="n">
         <f aca="false">$G$172</f>
@@ -10685,13 +10705,13 @@
         <v>20</v>
       </c>
       <c r="M181" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="N181" s="1" t="s">
         <v>43</v>
       </c>
       <c r="O181" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="R181" s="3" t="n">
         <f aca="false">R3</f>
@@ -10721,16 +10741,16 @@
     </row>
     <row r="182" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B182" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C182" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D182" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G182" s="1" t="n">
         <f aca="false">$G$172</f>
@@ -10751,13 +10771,13 @@
         <v>20</v>
       </c>
       <c r="M182" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="N182" s="1" t="s">
         <v>43</v>
       </c>
       <c r="O182" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="R182" s="3" t="n">
         <f aca="false">R3</f>
@@ -10787,16 +10807,16 @@
     </row>
     <row r="183" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B183" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C183" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D183" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G183" s="1" t="n">
         <f aca="false">$G$172</f>
@@ -10817,13 +10837,13 @@
         <v>20</v>
       </c>
       <c r="M183" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="N183" s="1" t="s">
         <v>43</v>
       </c>
       <c r="O183" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="R183" s="3" t="n">
         <f aca="false">R3</f>
@@ -10853,16 +10873,16 @@
     </row>
     <row r="184" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B184" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C184" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D184" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G184" s="1" t="n">
         <f aca="false">$G$172</f>
@@ -10883,13 +10903,13 @@
         <v>20</v>
       </c>
       <c r="M184" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="N184" s="1" t="s">
         <v>43</v>
       </c>
       <c r="O184" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="R184" s="3" t="n">
         <f aca="false">R3</f>
@@ -10919,16 +10939,16 @@
     </row>
     <row r="185" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B185" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C185" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D185" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G185" s="1" t="n">
         <f aca="false">$G$172</f>
@@ -10947,13 +10967,13 @@
         <v>20</v>
       </c>
       <c r="M185" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="N185" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="O185" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="R185" s="3" t="n">
         <f aca="false">R3</f>
@@ -10982,16 +11002,16 @@
     </row>
     <row r="186" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B186" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C186" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D186" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G186" s="1" t="n">
         <f aca="false">$G$172</f>
@@ -11012,13 +11032,13 @@
         <v>20</v>
       </c>
       <c r="M186" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="N186" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="O186" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="R186" s="3" t="n">
         <f aca="false">R3</f>
@@ -11048,16 +11068,16 @@
     </row>
     <row r="187" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B187" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C187" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D187" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G187" s="1" t="n">
         <f aca="false">$G$172</f>
@@ -11078,13 +11098,13 @@
         <v>20</v>
       </c>
       <c r="M187" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="N187" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="O187" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="R187" s="3" t="n">
         <f aca="false">R3</f>
@@ -11114,16 +11134,16 @@
     </row>
     <row r="188" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B188" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C188" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D188" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G188" s="1" t="n">
         <f aca="false">$G$172</f>
@@ -11144,13 +11164,13 @@
         <v>20</v>
       </c>
       <c r="M188" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="N188" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="O188" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="R188" s="3" t="n">
         <f aca="false">R3</f>
@@ -11180,16 +11200,16 @@
     </row>
     <row r="189" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B189" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C189" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D189" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G189" s="1" t="n">
         <f aca="false">$G$172</f>
@@ -11210,13 +11230,13 @@
         <v>20</v>
       </c>
       <c r="M189" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="N189" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="O189" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="R189" s="3" t="n">
         <f aca="false">R3</f>
@@ -11246,16 +11266,16 @@
     </row>
     <row r="190" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B190" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C190" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D190" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G190" s="1" t="n">
         <f aca="false">$G$172</f>
@@ -11276,13 +11296,13 @@
         <v>20</v>
       </c>
       <c r="M190" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="N190" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="O190" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="R190" s="3" t="n">
         <f aca="false">R3</f>
@@ -11312,16 +11332,16 @@
     </row>
     <row r="191" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B191" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C191" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D191" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G191" s="1" t="n">
         <f aca="false">$G$172</f>
@@ -11340,13 +11360,13 @@
         <v>20</v>
       </c>
       <c r="M191" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="N191" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="O191" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="R191" s="3" t="n">
         <f aca="false">R3</f>
@@ -11376,16 +11396,16 @@
     </row>
     <row r="192" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B192" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C192" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D192" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G192" s="1" t="n">
         <f aca="false">$G$172</f>
@@ -11406,13 +11426,13 @@
         <v>20</v>
       </c>
       <c r="M192" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="N192" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="O192" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="R192" s="3" t="n">
         <f aca="false">R3</f>
@@ -11442,16 +11462,16 @@
     </row>
     <row r="193" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B193" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C193" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D193" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G193" s="1" t="n">
         <f aca="false">$G$172</f>
@@ -11472,13 +11492,13 @@
         <v>20</v>
       </c>
       <c r="M193" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="N193" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="O193" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="R193" s="3" t="n">
         <f aca="false">R3</f>
@@ -11508,16 +11528,16 @@
     </row>
     <row r="194" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B194" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C194" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D194" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G194" s="1" t="n">
         <f aca="false">$G$172</f>
@@ -11538,13 +11558,13 @@
         <v>20</v>
       </c>
       <c r="M194" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="N194" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="O194" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="R194" s="3" t="n">
         <f aca="false">R3</f>
@@ -11574,16 +11594,16 @@
     </row>
     <row r="195" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B195" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C195" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D195" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G195" s="1" t="n">
         <f aca="false">$G$172</f>
@@ -11604,13 +11624,13 @@
         <v>20</v>
       </c>
       <c r="M195" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="N195" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="O195" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="R195" s="3" t="n">
         <f aca="false">R3</f>
@@ -11640,16 +11660,16 @@
     </row>
     <row r="196" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B196" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C196" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D196" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G196" s="1" t="n">
         <f aca="false">$G$172</f>
@@ -11670,13 +11690,13 @@
         <v>20</v>
       </c>
       <c r="M196" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="N196" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="O196" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="R196" s="3" t="n">
         <f aca="false">R3</f>
@@ -11706,16 +11726,16 @@
     </row>
     <row r="197" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B197" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C197" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D197" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G197" s="1" t="n">
         <f aca="false">$G$172</f>
@@ -11734,13 +11754,13 @@
         <v>20</v>
       </c>
       <c r="M197" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="N197" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="O197" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="R197" s="3" t="n">
         <f aca="false">R3</f>
@@ -11770,16 +11790,16 @@
     </row>
     <row r="198" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B198" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C198" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D198" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G198" s="1" t="n">
         <f aca="false">$G$172</f>
@@ -11800,13 +11820,13 @@
         <v>20</v>
       </c>
       <c r="M198" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="N198" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="O198" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="R198" s="3" t="n">
         <f aca="false">R3</f>
@@ -11836,16 +11856,16 @@
     </row>
     <row r="199" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B199" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C199" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D199" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G199" s="1" t="n">
         <f aca="false">$G$172</f>
@@ -11866,13 +11886,13 @@
         <v>20</v>
       </c>
       <c r="M199" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="N199" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="O199" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="R199" s="3" t="n">
         <f aca="false">R3</f>
@@ -11902,16 +11922,16 @@
     </row>
     <row r="200" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B200" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C200" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D200" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G200" s="1" t="n">
         <f aca="false">$G$172</f>
@@ -11932,13 +11952,13 @@
         <v>20</v>
       </c>
       <c r="M200" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="N200" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="O200" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="R200" s="3" t="n">
         <f aca="false">R3</f>
@@ -11968,16 +11988,16 @@
     </row>
     <row r="201" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B201" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C201" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D201" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G201" s="1" t="n">
         <f aca="false">$G$172</f>
@@ -11998,13 +12018,13 @@
         <v>20</v>
       </c>
       <c r="M201" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="N201" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="O201" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="R201" s="3" t="n">
         <f aca="false">R3</f>
@@ -12034,16 +12054,16 @@
     </row>
     <row r="202" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B202" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C202" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D202" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G202" s="1" t="n">
         <f aca="false">$G$172</f>
@@ -12064,13 +12084,13 @@
         <v>20</v>
       </c>
       <c r="M202" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="N202" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="O202" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="R202" s="3" t="n">
         <f aca="false">R3</f>
@@ -12100,16 +12120,16 @@
     </row>
     <row r="203" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B203" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C203" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D203" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G203" s="1" t="n">
         <f aca="false">$G$172</f>
@@ -12128,13 +12148,13 @@
         <v>20</v>
       </c>
       <c r="M203" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="N203" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="O203" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="R203" s="3" t="n">
         <f aca="false">R3</f>
@@ -12164,16 +12184,16 @@
     </row>
     <row r="204" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B204" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C204" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D204" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G204" s="1" t="n">
         <f aca="false">$G$172</f>
@@ -12194,13 +12214,13 @@
         <v>20</v>
       </c>
       <c r="M204" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="N204" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="O204" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="R204" s="3" t="n">
         <f aca="false">R3</f>
@@ -12230,16 +12250,16 @@
     </row>
     <row r="205" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B205" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C205" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D205" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G205" s="1" t="n">
         <f aca="false">$G$172</f>
@@ -12260,13 +12280,13 @@
         <v>20</v>
       </c>
       <c r="M205" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="N205" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="O205" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="R205" s="3" t="n">
         <f aca="false">R3</f>
@@ -12296,16 +12316,16 @@
     </row>
     <row r="206" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B206" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C206" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D206" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G206" s="1" t="n">
         <f aca="false">$G$172</f>
@@ -12326,13 +12346,13 @@
         <v>20</v>
       </c>
       <c r="M206" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="N206" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="O206" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="R206" s="3" t="n">
         <f aca="false">R3</f>
@@ -12362,16 +12382,16 @@
     </row>
     <row r="207" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B207" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C207" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D207" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G207" s="1" t="n">
         <f aca="false">$G$172</f>
@@ -12392,13 +12412,13 @@
         <v>20</v>
       </c>
       <c r="M207" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="N207" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="O207" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="R207" s="3" t="n">
         <f aca="false">R3</f>
@@ -12428,16 +12448,16 @@
     </row>
     <row r="208" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B208" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C208" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D208" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G208" s="1" t="n">
         <f aca="false">$G$172</f>
@@ -12458,13 +12478,13 @@
         <v>20</v>
       </c>
       <c r="M208" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="N208" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="O208" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="R208" s="3" t="n">
         <f aca="false">R3</f>

</xml_diff>